<commit_message>
Started implementing UV_Subtract function
</commit_message>
<xml_diff>
--- a/Testing Broad-Scale Interactions/Mini_Matrix_Test.xlsx
+++ b/Testing Broad-Scale Interactions/Mini_Matrix_Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Radicinol\Desktop\R\Testing Broad-Scale Interactions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9E2FE5B-D467-4578-A244-DFB1A6FFE26E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC89B535-EC75-4B06-8499-A29F8E82B516}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{03A45048-D6D3-4FA6-BE96-5E28A62A3FF2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>CON1</t>
   </si>
@@ -45,31 +45,13 @@
     <t>Coculture</t>
   </si>
   <si>
-    <t>F1CON</t>
-  </si>
-  <si>
-    <t>F2CON</t>
-  </si>
-  <si>
-    <t>F1vF2</t>
-  </si>
-  <si>
-    <t>F3CON</t>
-  </si>
-  <si>
-    <t>F1vF3</t>
-  </si>
-  <si>
-    <t>F2vF1</t>
-  </si>
-  <si>
-    <t>F2vF3</t>
-  </si>
-  <si>
-    <t>F3vF1</t>
-  </si>
-  <si>
-    <t>F3vF2</t>
+    <t>27CON</t>
+  </si>
+  <si>
+    <t>04CON</t>
+  </si>
+  <si>
+    <t>27v04</t>
   </si>
 </sst>
 </file>
@@ -430,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9BB15BF-964D-4F39-ADC2-D0329E190B17}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,61 +442,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Optimised UV check and various other paramaters following a manual check of the matched peaks
</commit_message>
<xml_diff>
--- a/Testing Broad-Scale Interactions/Mini_Matrix_Test.xlsx
+++ b/Testing Broad-Scale Interactions/Mini_Matrix_Test.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Radicinol\Desktop\R\Testing Broad-Scale Interactions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\43287069\Documents\GitHub\Microbial_Interactions\Testing Broad-Scale Interactions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC89B535-EC75-4B06-8499-A29F8E82B516}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{03A45048-D6D3-4FA6-BE96-5E28A62A3FF2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t>CON1</t>
   </si>
@@ -45,19 +44,37 @@
     <t>Coculture</t>
   </si>
   <si>
-    <t>27CON</t>
-  </si>
-  <si>
-    <t>04CON</t>
-  </si>
-  <si>
-    <t>27v04</t>
+    <t>F1CON</t>
+  </si>
+  <si>
+    <t>F2CON</t>
+  </si>
+  <si>
+    <t>F1vF2</t>
+  </si>
+  <si>
+    <t>F3CON</t>
+  </si>
+  <si>
+    <t>F1vF3</t>
+  </si>
+  <si>
+    <t>F2vF1</t>
+  </si>
+  <si>
+    <t>F2vF3</t>
+  </si>
+  <si>
+    <t>F3vF1</t>
+  </si>
+  <si>
+    <t>F3vF2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -411,11 +428,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9BB15BF-964D-4F39-ADC2-D0329E190B17}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,6 +459,61 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>